<commit_message>
pre setting match obs
</commit_message>
<xml_diff>
--- a/UploadStudentList_tid2.xlsx
+++ b/UploadStudentList_tid2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ALLForFYP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5BDD28-C0D6-4DA5-8681-4F310A7F1AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC54FF0-0AB3-48A2-90D4-3BE691B1E63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,27 +55,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>sid55555</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sid66666</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>spw55555</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>spw66666</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>how to get efg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>where is efg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sid21111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sid22222</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spw21111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spw22222</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -438,7 +438,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -468,13 +468,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -482,13 +482,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>